<commit_message>
Documentation and extra exception handling
</commit_message>
<xml_diff>
--- a/Optimisation_Spreadsheet.xlsx
+++ b/Optimisation_Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shakeelsubratty/PycharmProjects/optimisation/venv/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464BB1AB-F75C-B748-9337-1D2551431059}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863AEFF3-3BBA-4D4C-96FB-F1CDFF4B9965}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="1" xr2:uid="{5A44FB99-32D9-7941-96CE-1A742DBA76D8}"/>
   </bookViews>
@@ -4187,7 +4187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4199,6 +4199,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4537,7 +4540,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5367,8 +5370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9BA9D2-15BC-DE4B-B138-2CB506C7A197}">
   <dimension ref="A1:Q1235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5429,6 +5432,7 @@
       <c r="M1" s="2" t="s">
         <v>1359</v>
       </c>
+      <c r="O1" s="7"/>
       <c r="P1" s="2" t="s">
         <v>1361</v>
       </c>
@@ -5476,8 +5480,9 @@
       <c r="M2" s="5">
         <v>43677</v>
       </c>
+      <c r="O2" s="5"/>
       <c r="P2" s="5">
-        <v>43651</v>
+        <v>43672</v>
       </c>
       <c r="Q2" s="6">
         <v>840</v>
@@ -5523,8 +5528,9 @@
       <c r="M3" s="5">
         <v>43677</v>
       </c>
+      <c r="O3" s="5"/>
       <c r="P3" s="5">
-        <v>43652</v>
+        <v>43666</v>
       </c>
       <c r="Q3" s="6">
         <v>840</v>
@@ -5570,8 +5576,9 @@
       <c r="M4" s="5">
         <v>43671</v>
       </c>
+      <c r="O4" s="5"/>
       <c r="P4" s="5">
-        <v>43653</v>
+        <v>43660</v>
       </c>
       <c r="Q4" s="6">
         <v>840</v>
@@ -5617,8 +5624,9 @@
       <c r="M5" s="5">
         <v>43665</v>
       </c>
+      <c r="O5" s="5"/>
       <c r="P5" s="5">
-        <v>43656</v>
+        <v>43677</v>
       </c>
       <c r="Q5" s="6">
         <v>840</v>
@@ -5664,8 +5672,9 @@
       <c r="M6" s="5">
         <v>43665</v>
       </c>
+      <c r="O6" s="5"/>
       <c r="P6" s="5">
-        <v>43657</v>
+        <v>43667</v>
       </c>
       <c r="Q6" s="6">
         <v>840</v>
@@ -5711,8 +5720,9 @@
       <c r="M7" s="5">
         <v>43682</v>
       </c>
+      <c r="O7" s="5"/>
       <c r="P7" s="5">
-        <v>43658</v>
+        <v>43671</v>
       </c>
       <c r="Q7" s="6">
         <v>840</v>
@@ -5758,8 +5768,9 @@
       <c r="M8" s="5">
         <v>43672</v>
       </c>
+      <c r="O8" s="5"/>
       <c r="P8" s="5">
-        <v>43659</v>
+        <v>43673</v>
       </c>
       <c r="Q8" s="6">
         <v>840</v>
@@ -5805,8 +5816,9 @@
       <c r="M9" s="5">
         <v>43682</v>
       </c>
+      <c r="O9" s="5"/>
       <c r="P9" s="5">
-        <v>43660</v>
+        <v>43664</v>
       </c>
       <c r="Q9" s="6">
         <v>840</v>
@@ -5852,8 +5864,9 @@
       <c r="M10" s="5">
         <v>43671</v>
       </c>
+      <c r="O10" s="5"/>
       <c r="P10" s="5">
-        <v>43663</v>
+        <v>43657</v>
       </c>
       <c r="Q10" s="6">
         <v>840</v>
@@ -5899,8 +5912,9 @@
       <c r="M11" s="5">
         <v>43672</v>
       </c>
+      <c r="O11" s="5"/>
       <c r="P11" s="5">
-        <v>43664</v>
+        <v>43656</v>
       </c>
       <c r="Q11" s="6">
         <v>840</v>
@@ -5946,6 +5960,7 @@
       <c r="M12" s="5">
         <v>43677</v>
       </c>
+      <c r="O12" s="5"/>
       <c r="P12" s="5">
         <v>43665</v>
       </c>
@@ -5993,8 +6008,9 @@
       <c r="M13" s="5">
         <v>43677</v>
       </c>
+      <c r="O13" s="5"/>
       <c r="P13" s="5">
-        <v>43666</v>
+        <v>43670</v>
       </c>
       <c r="Q13" s="6">
         <v>840</v>
@@ -6040,8 +6056,9 @@
       <c r="M14" s="5">
         <v>43671</v>
       </c>
+      <c r="O14" s="5"/>
       <c r="P14" s="5">
-        <v>43667</v>
+        <v>43653</v>
       </c>
       <c r="Q14" s="6">
         <v>1140</v>
@@ -6087,8 +6104,9 @@
       <c r="M15" s="5">
         <v>43671</v>
       </c>
+      <c r="O15" s="5"/>
       <c r="P15" s="5">
-        <v>43670</v>
+        <v>43663</v>
       </c>
       <c r="Q15" s="6">
         <v>840</v>
@@ -6134,8 +6152,9 @@
       <c r="M16" s="5">
         <v>43672</v>
       </c>
+      <c r="O16" s="5"/>
       <c r="P16" s="5">
-        <v>43671</v>
+        <v>43651</v>
       </c>
       <c r="Q16" s="6">
         <v>840</v>
@@ -6181,8 +6200,9 @@
       <c r="M17" s="5">
         <v>43676</v>
       </c>
+      <c r="O17" s="5"/>
       <c r="P17" s="5">
-        <v>43672</v>
+        <v>43652</v>
       </c>
       <c r="Q17" s="6">
         <v>1140</v>
@@ -6228,8 +6248,9 @@
       <c r="M18" s="5">
         <v>43677</v>
       </c>
+      <c r="O18" s="5"/>
       <c r="P18" s="5">
-        <v>43673</v>
+        <v>43659</v>
       </c>
       <c r="Q18" s="6">
         <v>840</v>
@@ -6275,8 +6296,9 @@
       <c r="M19" s="5">
         <v>43677</v>
       </c>
+      <c r="O19" s="5"/>
       <c r="P19" s="5">
-        <v>43674</v>
+        <v>43658</v>
       </c>
       <c r="Q19" s="6">
         <v>840</v>
@@ -6322,8 +6344,9 @@
       <c r="M20" s="5">
         <v>43671</v>
       </c>
+      <c r="O20" s="5"/>
       <c r="P20" s="5">
-        <v>43677</v>
+        <v>43674</v>
       </c>
       <c r="Q20" s="6">
         <v>840</v>
@@ -55684,7 +55707,7 @@
         <v>0.25</v>
       </c>
       <c r="K1218">
-        <f t="shared" ref="K1218:K1281" si="59">ROUND(PRODUCT(J1218,60),0)</f>
+        <f t="shared" ref="K1218:K1235" si="59">ROUND(PRODUCT(J1218,60),0)</f>
         <v>15</v>
       </c>
       <c r="L1218" t="s">
@@ -56395,7 +56418,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F1235" xr:uid="{07999850-C0AD-F24A-B05C-56E97B6E2F0B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P2:P21">
     <sortCondition ref="P1"/>
   </sortState>

</xml_diff>